<commit_message>
Updating Filter Data table
</commit_message>
<xml_diff>
--- a/HighSalary/HighEmpSalary.xlsx
+++ b/HighSalary/HighEmpSalary.xlsx
@@ -1,77 +1,404 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <x:workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d6ae4885f7a20e84/Documents/UiPath/Natwest_Employee_Salary_Update/HighSalary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A55F8EB8-57BD-407D-B03D-899E682AF389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{06332DCB-EC80-4EA4-BDD1-65FB7EE3035D}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{A55F8EB8-57BD-407D-B03D-899E682AF389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3202E6BE-341F-4A09-8450-B6448BC7EEC0}"/>
+  <x:bookViews>
+    <x:workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="0" activeTab="0" xr2:uid="{06332DCB-EC80-4EA4-BDD1-65FB7EE3035D}"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="191029"/>
+  <x:extLst>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
-</workbook>
+    </x:ext>
+  </x:extLst>
+</x:workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:si>
+    <x:t>2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ajay</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>uipath</x:t>
+  </x:si>
+  <x:si>
+    <x:t>25000</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Kunal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>AIML</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20000</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dick</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30000</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Harry</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>python</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15000</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Rahul</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Lucky</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Nisha</x:t>
+  </x:si>
+  <x:si>
+    <x:t>10</x:t>
+  </x:si>
+  <x:si>
+    <x:t>40000</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Payal</x:t>
+  </x:si>
+  <x:si>
+    <x:t>15</x:t>
+  </x:si>
+  <x:si>
+    <x:t>11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Roma</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Raj</x:t>
+  </x:si>
+  <x:si>
+    <x:t>13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Shankar</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Amit</x:t>
+  </x:si>
+  <x:si>
+    <x:t>16</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vidit</x:t>
+  </x:si>
+  <x:si>
+    <x:t>18</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Karmit</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Harmit</x:t>
+  </x:si>
+  <x:si>
+    <x:t>20</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Deepa</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac x16r2 xr">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="2" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  </x:cellStyleXfs>
+  <x:cellXfs count="1">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+    </x:ext>
+    <x:ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
       <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$16:$D$16</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Deepa</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>uipath</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$E$1:$E$15</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15000</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F723-4B73-BDD8-296DE6603040}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{03FB9D22-9AD1-AC5E-0BA5-F472B9989964}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -370,13 +697,294 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4AB4163-2D76-473A-91F4-CB961D7FDC6D}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xr:uid="{F4AB4163-2D76-473A-91F4-CB961D7FDC6D}" mc:Ignorable="x14ac xr xr2 xr3">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:E16"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <x:c r="A1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <x:c r="A2" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B2" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <x:c r="A3" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <x:c r="A4" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <x:c r="A5" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <x:c r="A6" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <x:c r="A7" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <x:c r="A8" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <x:c r="A9" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <x:c r="A10" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <x:c r="A11" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="B11" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="C11" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="D11" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E11" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <x:c r="A12" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B12" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="C12" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D12" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E12" s="0" t="s">
+        <x:v>9</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <x:c r="A13" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="B13" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="C13" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="D13" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E13" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <x:c r="A14" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="B14" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="C14" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="D14" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E14" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <x:c r="A15" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="B15" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="C15" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <x:c r="A16" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="B16" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="C16" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D16" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E16" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:drawing r:id="rId1"/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>